<commit_message>
Update a bunch of files (all main scripts except 101, 109, 111)
</commit_message>
<xml_diff>
--- a/Input_data/EQS_limits.xlsx
+++ b/Input_data/EQS_limits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\seksjon 212\Milkys\Input_data\Data_limits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHJ\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3CCC24-D309-4FD2-A5A3-AF5E5AD78E3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1A6E2F-8500-4116-809A-38BEB9EF219E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EQS" sheetId="2" r:id="rId1"/>
@@ -923,7 +923,7 @@
     <t>D5</t>
   </si>
   <si>
-    <t>TPTIN</t>
+    <t>TPT</t>
   </si>
 </sst>
 </file>
@@ -1864,22 +1864,22 @@
   <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" customWidth="1"/>
+    <col min="2" max="3" width="7.41796875" customWidth="1"/>
+    <col min="4" max="4" width="3.68359375" customWidth="1"/>
+    <col min="5" max="5" width="25.26171875" customWidth="1"/>
+    <col min="6" max="6" width="14.41796875" customWidth="1"/>
+    <col min="7" max="7" width="13.578125" customWidth="1"/>
     <col min="8" max="8" width="6" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="16" t="s">
         <v>173</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="K1" s="18"/>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>9</v>
       </c>
@@ -1953,7 +1953,7 @@
       <c r="T2" s="44"/>
       <c r="U2" s="44"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4">
         <v>11</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5">
         <v>11</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6">
         <v>12</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7">
         <v>13</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8">
         <v>14</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9">
         <v>15</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10">
         <v>16</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11">
         <v>17</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12">
         <v>18</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>19</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="E13" s="50"/>
       <c r="F13" s="51"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14">
         <v>20</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15">
         <v>21</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16">
         <v>22</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17">
         <v>23</v>
       </c>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="F17" s="43"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18">
         <v>24</v>
       </c>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="F18" s="43"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A19">
         <v>25</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A20">
         <v>26</v>
       </c>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="F20" s="43"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21">
         <v>27</v>
       </c>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="F21" s="43"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A22">
         <v>28</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A23">
         <v>28</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A24">
         <v>29</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25">
         <v>29</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A26">
         <v>30</v>
       </c>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="F26" s="43"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A27">
         <v>31</v>
       </c>
@@ -2504,7 +2504,7 @@
       </c>
       <c r="F27" s="43"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A28">
         <v>32</v>
       </c>
@@ -2516,7 +2516,7 @@
       </c>
       <c r="F28" s="43"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29">
         <v>33</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A30">
         <v>34</v>
       </c>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="F30" s="43"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A31">
         <v>35</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32">
         <v>36</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A33">
         <v>37</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34">
         <v>38</v>
       </c>
@@ -2665,7 +2665,7 @@
       <c r="S34" s="44"/>
       <c r="T34" s="44"/>
     </row>
-    <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35">
         <v>39</v>
       </c>
@@ -2704,7 +2704,7 @@
       <c r="S35" s="44"/>
       <c r="T35" s="44"/>
     </row>
-    <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A36">
         <v>38</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="S36" s="44"/>
       <c r="T36" s="44"/>
     </row>
-    <row r="37" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A37">
         <v>39</v>
       </c>
@@ -2785,7 +2785,7 @@
       <c r="S37" s="44"/>
       <c r="T37" s="44"/>
     </row>
-    <row r="38" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A38">
         <v>40</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A39">
         <v>41</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>42</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A41">
         <v>43</v>
       </c>
@@ -2863,7 +2863,7 @@
       </c>
       <c r="F41" s="46"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>44</v>
       </c>
@@ -2875,7 +2875,7 @@
       </c>
       <c r="F42" s="55"/>
     </row>
-    <row r="43" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A43">
         <v>45</v>
       </c>
@@ -2887,7 +2887,7 @@
       </c>
       <c r="F43" s="46"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>46</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>47</v>
       </c>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="F45" s="57"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>48</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A47">
         <v>49</v>
       </c>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="F47" s="60"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>50</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>51</v>
       </c>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="F49" s="57"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>52</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A51">
         <v>53</v>
       </c>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="F51" s="60"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>54</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A53">
         <v>55</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>56</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A55">
         <v>57</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>58</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A57">
         <v>59</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>60</v>
       </c>
@@ -3130,7 +3130,7 @@
       </c>
       <c r="F58" s="53"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>61</v>
       </c>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="F59" s="57"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>62</v>
       </c>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="F60" s="61"/>
     </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A61">
         <v>63</v>
       </c>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="F61" s="62"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>64</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A63">
         <v>65</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>66</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A65">
         <v>67</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>68</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A67">
         <v>69</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>70</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A69">
         <v>71</v>
       </c>
@@ -3320,7 +3320,7 @@
       <c r="L69" s="59"/>
       <c r="M69" s="59"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>72</v>
       </c>
@@ -3332,7 +3332,7 @@
       </c>
       <c r="F70" s="55"/>
     </row>
-    <row r="71" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A71">
         <v>73</v>
       </c>
@@ -3344,7 +3344,7 @@
       </c>
       <c r="F71" s="46"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <v>74</v>
       </c>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="F72" s="53"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
         <v>75</v>
       </c>
@@ -3364,7 +3364,7 @@
       <c r="E73" s="34"/>
       <c r="F73" s="57"/>
     </row>
-    <row r="74" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A74">
         <v>76</v>
       </c>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="F74" s="46"/>
     </row>
-    <row r="75" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A75">
         <v>77</v>
       </c>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="F75" s="46"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>78</v>
       </c>
@@ -3398,7 +3398,7 @@
       </c>
       <c r="F76" s="55"/>
     </row>
-    <row r="77" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A77">
         <v>79</v>
       </c>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="F77" s="66"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <v>80</v>
       </c>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="F78" s="67"/>
     </row>
-    <row r="79" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A79">
         <v>81</v>
       </c>
@@ -3428,7 +3428,7 @@
       </c>
       <c r="F79" s="66"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
         <v>82</v>
       </c>
@@ -3438,7 +3438,7 @@
       </c>
       <c r="F80" s="67"/>
     </row>
-    <row r="81" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A81">
         <v>83</v>
       </c>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="F81" s="66"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
         <v>84</v>
       </c>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="F82" s="67"/>
     </row>
-    <row r="83" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A83">
         <v>85</v>
       </c>
@@ -3468,7 +3468,7 @@
       </c>
       <c r="F83" s="66"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A84">
         <v>86</v>
       </c>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="F84" s="67"/>
     </row>
-    <row r="85" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A85">
         <v>87</v>
       </c>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="F85" s="66"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
         <v>88</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A87">
         <v>89</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
         <v>90</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="T88"/>
       <c r="U88"/>
     </row>
-    <row r="89" spans="1:21" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A89">
         <v>91</v>
       </c>
@@ -3579,7 +3579,7 @@
       <c r="T89"/>
       <c r="U89"/>
     </row>
-    <row r="90" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90">
         <v>92</v>
       </c>
@@ -3605,7 +3605,7 @@
       <c r="T90"/>
       <c r="U90"/>
     </row>
-    <row r="91" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91">
         <v>93</v>
       </c>
@@ -3631,7 +3631,7 @@
       <c r="T91"/>
       <c r="U91"/>
     </row>
-    <row r="92" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92">
         <v>94</v>
       </c>
@@ -3655,7 +3655,7 @@
       <c r="T92"/>
       <c r="U92"/>
     </row>
-    <row r="93" spans="1:21" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A93">
         <v>95</v>
       </c>
@@ -3681,7 +3681,7 @@
       <c r="T93"/>
       <c r="U93"/>
     </row>
-    <row r="94" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94">
         <v>96</v>
       </c>
@@ -3709,7 +3709,7 @@
       <c r="T94"/>
       <c r="U94"/>
     </row>
-    <row r="95" spans="1:21" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A95">
         <v>97</v>
       </c>
@@ -3737,7 +3737,7 @@
       <c r="T95"/>
       <c r="U95"/>
     </row>
-    <row r="96" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96">
         <v>98</v>
       </c>
@@ -3765,7 +3765,7 @@
       <c r="T96"/>
       <c r="U96"/>
     </row>
-    <row r="97" spans="1:21" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A97">
         <v>99</v>
       </c>
@@ -3795,7 +3795,7 @@
       <c r="T97"/>
       <c r="U97"/>
     </row>
-    <row r="98" spans="1:21" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" s="3" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A98">
         <v>100</v>
       </c>
@@ -3829,7 +3829,7 @@
       <c r="T98"/>
       <c r="U98"/>
     </row>
-    <row r="99" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99">
         <v>101</v>
       </c>
@@ -3859,7 +3859,7 @@
       <c r="T99"/>
       <c r="U99"/>
     </row>
-    <row r="100" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100">
         <v>102</v>
       </c>
@@ -3900,41 +3900,41 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="39.28515625" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="42.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.83984375" style="1"/>
+    <col min="2" max="2" width="7.68359375" customWidth="1"/>
+    <col min="3" max="3" width="9.15625" customWidth="1"/>
+    <col min="4" max="4" width="7.41796875" customWidth="1"/>
+    <col min="5" max="5" width="3.68359375" customWidth="1"/>
+    <col min="6" max="6" width="25.26171875" customWidth="1"/>
+    <col min="7" max="8" width="14.41796875" customWidth="1"/>
+    <col min="9" max="9" width="39.26171875" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="42.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="E5" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:13" s="9" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="9" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8"/>
       <c r="E7" s="77" t="s">
         <v>3</v>
@@ -3948,12 +3948,12 @@
       <c r="L7" s="77"/>
       <c r="M7" s="77"/>
     </row>
-    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F8" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="11" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="11" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="8"/>
       <c r="F9" s="78" t="s">
         <v>5</v>
@@ -3966,7 +3966,7 @@
       <c r="L9" s="78"/>
       <c r="M9" s="78"/>
     </row>
-    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F10" s="10"/>
       <c r="K10" t="e">
         <f ca="1">Fillcolor(L10)</f>
@@ -3976,7 +3976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E12" s="79" t="s">
         <v>9</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="F13" s="10"/>
       <c r="K13" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -4015,7 +4015,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" s="19" t="s">
         <v>20</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="24" t="s">
@@ -4135,7 +4135,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C18" t="s">
         <v>29</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="G19" s="32"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
         <v>34</v>
       </c>
@@ -4187,7 +4187,7 @@
       </c>
       <c r="G20" s="35"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
         <v>34</v>
       </c>
@@ -4200,7 +4200,7 @@
       </c>
       <c r="G21" s="36"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
         <v>34</v>
       </c>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="G22" s="36"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="G23" s="36"/>
     </row>
-    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B24" t="s">
         <v>34</v>
       </c>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="G24" s="36"/>
     </row>
-    <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B25" t="s">
         <v>34</v>
       </c>
@@ -4254,7 +4254,7 @@
       </c>
       <c r="G25" s="39"/>
     </row>
-    <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B26" t="s">
         <v>34</v>
       </c>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="G26" s="42"/>
     </row>
-    <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
@@ -4313,7 +4313,7 @@
       <c r="U27" s="44"/>
       <c r="V27" s="44"/>
     </row>
-    <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A37" s="1" t="s">
         <v>18</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" t="s">
         <v>34</v>
       </c>
@@ -4611,7 +4611,7 @@
       <c r="F38" s="50"/>
       <c r="G38" s="51"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A39" s="1" t="s">
         <v>18</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A40" s="1" t="s">
         <v>18</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A41" s="1" t="s">
         <v>18</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B42" t="s">
         <v>34</v>
       </c>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="G42" s="43"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B43" t="s">
         <v>34</v>
       </c>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="G43" s="43"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B45" t="s">
         <v>34</v>
       </c>
@@ -4769,7 +4769,7 @@
       </c>
       <c r="G45" s="43"/>
     </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B46" t="s">
         <v>34</v>
       </c>
@@ -4784,7 +4784,7 @@
       </c>
       <c r="G46" s="43"/>
     </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A47" s="1" t="s">
         <v>18</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A48" s="1" t="s">
         <v>18</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A49" s="1" t="s">
         <v>18</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A50" s="1" t="s">
         <v>18</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B51" t="s">
         <v>34</v>
       </c>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="G51" s="43"/>
     </row>
-    <row r="52" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B52" t="s">
         <v>34</v>
       </c>
@@ -4942,7 +4942,7 @@
       </c>
       <c r="G52" s="43"/>
     </row>
-    <row r="53" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B53" t="s">
         <v>34</v>
       </c>
@@ -4957,7 +4957,7 @@
       </c>
       <c r="G53" s="43"/>
     </row>
-    <row r="54" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A54" s="1" t="s">
         <v>18</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B55" t="s">
         <v>34</v>
       </c>
@@ -4998,7 +4998,7 @@
       </c>
       <c r="G55" s="43"/>
     </row>
-    <row r="56" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A56" s="1" t="s">
         <v>18</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A57" s="1" t="s">
         <v>18</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A58" s="1" t="s">
         <v>18</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A59" s="1" t="s">
         <v>18</v>
       </c>
@@ -5130,7 +5130,7 @@
       <c r="T59" s="44"/>
       <c r="U59" s="44"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A60" s="1" t="s">
         <v>18</v>
       </c>
@@ -5172,7 +5172,7 @@
       <c r="T60" s="44"/>
       <c r="U60" s="44"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A61" s="1" t="s">
         <v>18</v>
       </c>
@@ -5217,7 +5217,7 @@
       <c r="T61" s="44"/>
       <c r="U61" s="44"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A62" s="1" t="s">
         <v>18</v>
       </c>
@@ -5259,7 +5259,7 @@
       <c r="T62" s="44"/>
       <c r="U62" s="44"/>
     </row>
-    <row r="63" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B63" t="s">
         <v>34</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B64" t="s">
         <v>34</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" t="s">
         <v>116</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="66" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B66" t="s">
         <v>116</v>
       </c>
@@ -5343,7 +5343,7 @@
       </c>
       <c r="G66" s="46"/>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" t="s">
         <v>116</v>
       </c>
@@ -5358,7 +5358,7 @@
       </c>
       <c r="G67" s="55"/>
     </row>
-    <row r="68" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B68" t="s">
         <v>116</v>
       </c>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="G68" s="46"/>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B69" t="s">
         <v>116</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B70" t="s">
         <v>116</v>
       </c>
@@ -5403,7 +5403,7 @@
       </c>
       <c r="G70" s="57"/>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B71" t="s">
         <v>116</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B72" t="s">
         <v>116</v>
       </c>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="G72" s="60"/>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B73" t="s">
         <v>116</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" t="s">
         <v>116</v>
       </c>
@@ -5472,7 +5472,7 @@
       </c>
       <c r="G74" s="57"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" t="s">
         <v>116</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B76" t="s">
         <v>116</v>
       </c>
@@ -5508,7 +5508,7 @@
       </c>
       <c r="G76" s="60"/>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" t="s">
         <v>116</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B78" t="s">
         <v>116</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" t="s">
         <v>116</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="80" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B80" t="s">
         <v>116</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B81" t="s">
         <v>116</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="82" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B82" t="s">
         <v>116</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B83" t="s">
         <v>116</v>
       </c>
@@ -5655,7 +5655,7 @@
       </c>
       <c r="G83" s="53"/>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" t="s">
         <v>116</v>
       </c>
@@ -5668,7 +5668,7 @@
       </c>
       <c r="G84" s="57"/>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B85" t="s">
         <v>116</v>
       </c>
@@ -5683,7 +5683,7 @@
       </c>
       <c r="G85" s="61"/>
     </row>
-    <row r="86" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B86" t="s">
         <v>116</v>
       </c>
@@ -5696,7 +5696,7 @@
       </c>
       <c r="G86" s="62"/>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B87" t="s">
         <v>116</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="88" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B88" t="s">
         <v>116</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B89" t="s">
         <v>116</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="90" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B90" t="s">
         <v>116</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B91" t="s">
         <v>116</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="92" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B92" t="s">
         <v>116</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B93" t="s">
         <v>116</v>
       </c>
@@ -5839,7 +5839,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="94" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B94" t="s">
         <v>116</v>
       </c>
@@ -5872,7 +5872,7 @@
       <c r="M94" s="59"/>
       <c r="N94" s="59"/>
     </row>
-    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B95" t="s">
         <v>116</v>
       </c>
@@ -5887,7 +5887,7 @@
       </c>
       <c r="G95" s="55"/>
     </row>
-    <row r="96" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B96" t="s">
         <v>116</v>
       </c>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="G96" s="46"/>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B97" t="s">
         <v>116</v>
       </c>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="G97" s="53"/>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B98" t="s">
         <v>116</v>
       </c>
@@ -5928,7 +5928,7 @@
       <c r="F98" s="34"/>
       <c r="G98" s="57"/>
     </row>
-    <row r="99" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B99" t="s">
         <v>116</v>
       </c>
@@ -5943,7 +5943,7 @@
       </c>
       <c r="G99" s="46"/>
     </row>
-    <row r="100" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B100" t="s">
         <v>116</v>
       </c>
@@ -5958,7 +5958,7 @@
       </c>
       <c r="G100" s="46"/>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B101" t="s">
         <v>116</v>
       </c>
@@ -5971,7 +5971,7 @@
       </c>
       <c r="G101" s="55"/>
     </row>
-    <row r="102" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B102" t="s">
         <v>116</v>
       </c>
@@ -5984,7 +5984,7 @@
       </c>
       <c r="G102" s="66"/>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B103" t="s">
         <v>116</v>
       </c>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="G103" s="67"/>
     </row>
-    <row r="104" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B104" t="s">
         <v>116</v>
       </c>
@@ -6010,7 +6010,7 @@
       </c>
       <c r="G104" s="66"/>
     </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B105" t="s">
         <v>116</v>
       </c>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="G105" s="67"/>
     </row>
-    <row r="106" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B106" t="s">
         <v>116</v>
       </c>
@@ -6036,7 +6036,7 @@
       </c>
       <c r="G106" s="66"/>
     </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B107" t="s">
         <v>116</v>
       </c>
@@ -6049,7 +6049,7 @@
       </c>
       <c r="G107" s="67"/>
     </row>
-    <row r="108" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B108" t="s">
         <v>116</v>
       </c>
@@ -6062,7 +6062,7 @@
       </c>
       <c r="G108" s="66"/>
     </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B109" t="s">
         <v>116</v>
       </c>
@@ -6075,7 +6075,7 @@
       </c>
       <c r="G109" s="67"/>
     </row>
-    <row r="110" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B110" t="s">
         <v>116</v>
       </c>
@@ -6088,7 +6088,7 @@
       </c>
       <c r="G110" s="66"/>
     </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B111" t="s">
         <v>116</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="112" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B112" t="s">
         <v>116</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B113" t="s">
         <v>116</v>
       </c>
@@ -6143,7 +6143,7 @@
       </c>
       <c r="G113" s="67"/>
     </row>
-    <row r="114" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B114" t="s">
         <v>116</v>
       </c>
@@ -6156,7 +6156,7 @@
       </c>
       <c r="G114" s="66"/>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B115" t="s">
         <v>116</v>
       </c>
@@ -6169,7 +6169,7 @@
       </c>
       <c r="G115" s="73"/>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B116" t="s">
         <v>116</v>
       </c>
@@ -6182,7 +6182,7 @@
       </c>
       <c r="G116" s="74"/>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B117" t="s">
         <v>116</v>
       </c>
@@ -6193,7 +6193,7 @@
       <c r="F117" s="75"/>
       <c r="G117" s="74"/>
     </row>
-    <row r="118" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B118" t="s">
         <v>116</v>
       </c>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="G118" s="66"/>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B119" t="s">
         <v>116</v>
       </c>
@@ -6221,7 +6221,7 @@
       </c>
       <c r="G119" s="67"/>
     </row>
-    <row r="120" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B120" t="s">
         <v>116</v>
       </c>
@@ -6236,7 +6236,7 @@
       </c>
       <c r="G120" s="66"/>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B121" t="s">
         <v>116</v>
       </c>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="G121" s="67"/>
     </row>
-    <row r="122" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B122" t="s">
         <v>168</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B123" t="s">
         <v>168</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B124" t="s">
         <v>168</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>6.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B125" t="s">
         <v>168</v>
       </c>

</xml_diff>

<commit_message>
Update PROREF and EQS files with TPhT
- also save 'proref_used.csv'
</commit_message>
<xml_diff>
--- a/Input_data/EQS_limits.xlsx
+++ b/Input_data/EQS_limits.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHJ\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1A6E2F-8500-4116-809A-38BEB9EF219E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CD1AD7-2076-4AF5-B876-8327DF1B7F97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EQS" sheetId="2" r:id="rId1"/>
-    <sheet name="Extract for EQS - Arp-grenser" sheetId="1" r:id="rId2"/>
+    <sheet name="Changes" sheetId="3" r:id="rId2"/>
+    <sheet name="Extract for EQS - Arp-grenser" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EQS!$A$1:$J$98</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Extract for EQS - Arp-grenser'!$A$14:$K$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Extract for EQS - Arp-grenser'!$A$14:$K$123</definedName>
     <definedName name="_Ref397333801" localSheetId="0">EQS!#REF!</definedName>
-    <definedName name="_Ref397333801" localSheetId="1">'Extract for EQS - Arp-grenser'!$E$7</definedName>
+    <definedName name="_Ref397333801" localSheetId="2">'Extract for EQS - Arp-grenser'!$E$7</definedName>
     <definedName name="_Toc399230352" localSheetId="0">EQS!#REF!</definedName>
-    <definedName name="_Toc399230352" localSheetId="1">'Extract for EQS - Arp-grenser'!$E$4</definedName>
+    <definedName name="_Toc399230352" localSheetId="2">'Extract for EQS - Arp-grenser'!$E$4</definedName>
     <definedName name="_Toc399230353" localSheetId="0">EQS!#REF!</definedName>
-    <definedName name="_Toc399230353" localSheetId="1">'Extract for EQS - Arp-grenser'!$E$5</definedName>
+    <definedName name="_Toc399230353" localSheetId="2">'Extract for EQS - Arp-grenser'!$E$5</definedName>
     <definedName name="_Toc399230354" localSheetId="0">EQS!#REF!</definedName>
-    <definedName name="_Toc399230354" localSheetId="1">'Extract for EQS - Arp-grenser'!$E$11</definedName>
+    <definedName name="_Toc399230354" localSheetId="2">'Extract for EQS - Arp-grenser'!$E$11</definedName>
     <definedName name="EQStest" localSheetId="0">#REF!</definedName>
     <definedName name="EQStest">#REF!</definedName>
     <definedName name="piedata">#N/A</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="184">
   <si>
     <t>Fra Arp et al. (2014)</t>
   </si>
@@ -923,7 +924,16 @@
     <t>D5</t>
   </si>
   <si>
-    <t>TPT</t>
+    <t>TPhT</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>TPT changed to TPhT</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1544,6 +1554,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1863,7 +1874,7 @@
   </sheetPr>
   <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
@@ -3890,6 +3901,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEE71B8-15AF-44ED-8835-E0D6F6A5D2CC}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.15625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="80">
+        <v>44482</v>
+      </c>
+      <c r="B2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>

</xml_diff>